<commit_message>
Update tutorial to use safe division
</commit_message>
<xml_diff>
--- a/docs/tutorial/assets/t4_framework_1.xlsx
+++ b/docs/tutorial/assets/t4_framework_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\docs\tutorial\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh.abey\Desktop\projects\atomica\docs\tutorial\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBFB77D-5B96-4C51-8E75-A70F2D208869}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D057F5-8EC3-4B51-AA29-DBB274CF0913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21225" windowHeight="17085" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18900" windowHeight="10815" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
@@ -3155,9 +3155,6 @@
     <t>sus+inf+rec</t>
   </si>
   <si>
-    <t>infx*inf/popsize</t>
-  </si>
-  <si>
     <t>contacts</t>
   </si>
   <si>
@@ -3189,6 +3186,9 @@
   </si>
   <si>
     <t>inf,rec</t>
+  </si>
+  <si>
+    <t>infx*sdiv(inf,popsize)</t>
   </si>
 </sst>
 </file>
@@ -3925,7 +3925,7 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -8193,13 +8193,13 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -8213,13 +8213,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" t="s">
         <v>84</v>
-      </c>
-      <c r="C3" t="s">
-        <v>85</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>25</v>
@@ -8227,16 +8227,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>25</v>
@@ -8301,8 +8301,8 @@
   </sheetPr>
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8443,7 +8443,7 @@
         <v>63</v>
       </c>
       <c r="H5" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -8457,7 +8457,7 @@
         <v>63</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -8610,10 +8610,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>76</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>